<commit_message>
Put products in the database function, unit tests for all functions, database schema
</commit_message>
<xml_diff>
--- a/proj_aged/core/aged/lab/DataSafeOnes/01_good_AgedStock.xlsx
+++ b/proj_aged/core/aged/lab/DataSafeOnes/01_good_AgedStock.xlsx
@@ -1326,11 +1326,13 @@
   <dimension ref="A1:J233"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.34375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.35546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.16"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
functional tests for salespeople xlsx upload
</commit_message>
<xml_diff>
--- a/proj_aged/core/aged/lab/DataSafeOnes/01_good_AgedStock.xlsx
+++ b/proj_aged/core/aged/lab/DataSafeOnes/01_good_AgedStock.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="395">
   <si>
     <t xml:space="preserve">Plnt</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">CHO-006-160</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ta</t>
   </si>
   <si>
     <t xml:space="preserve">96_FU:811NVFAIR-01B_HK buttons 10KG/UC 2</t>
@@ -1325,11 +1328,11 @@
   </sheetPr>
   <dimension ref="A1:J233"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G224" activeCellId="0" sqref="G224"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.35546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.37109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.47"/>
@@ -1551,13 +1554,13 @@
         <v>1640</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>45566</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1568,7 +1571,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>13</v>
@@ -1600,7 +1603,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>13</v>
@@ -1632,7 +1635,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>13</v>
@@ -1653,7 +1656,7 @@
         <v>45645</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1664,7 +1667,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>13</v>
@@ -1685,7 +1688,7 @@
         <v>45693</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1696,10 +1699,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>14</v>
@@ -1717,7 +1720,7 @@
         <v>45593</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1728,10 +1731,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>14</v>
@@ -1749,7 +1752,7 @@
         <v>45633</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1760,13 +1763,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>62931743</v>
@@ -1781,7 +1784,7 @@
         <v>45581</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1792,13 +1795,13 @@
         <v>11</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>86697483</v>
@@ -1813,7 +1816,7 @@
         <v>45680</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1824,7 +1827,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>13</v>
@@ -1845,7 +1848,7 @@
         <v>45574</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1856,7 +1859,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>13</v>
@@ -1877,7 +1880,7 @@
         <v>45611</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1888,10 +1891,10 @@
         <v>11</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>14</v>
@@ -1909,7 +1912,7 @@
         <v>45603</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1920,10 +1923,10 @@
         <v>11</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>14</v>
@@ -1941,7 +1944,7 @@
         <v>45692</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1952,7 +1955,7 @@
         <v>11</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>13</v>
@@ -1973,7 +1976,7 @@
         <v>45655</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1984,7 +1987,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>13</v>
@@ -2005,7 +2008,7 @@
         <v>45523</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2016,10 +2019,10 @@
         <v>11</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>14</v>
@@ -2037,7 +2040,7 @@
         <v>45641</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2048,10 +2051,10 @@
         <v>11</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>14</v>
@@ -2069,7 +2072,7 @@
         <v>45707</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2080,10 +2083,10 @@
         <v>11</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>14</v>
@@ -2101,7 +2104,7 @@
         <v>45672</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2112,10 +2115,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>14</v>
@@ -2133,7 +2136,7 @@
         <v>45501</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2144,7 +2147,7 @@
         <v>11</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>13</v>
@@ -2165,7 +2168,7 @@
         <v>45712</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2176,10 +2179,10 @@
         <v>11</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>14</v>
@@ -2197,7 +2200,7 @@
         <v>45594</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2208,10 +2211,10 @@
         <v>11</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>14</v>
@@ -2229,7 +2232,7 @@
         <v>45735</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2240,10 +2243,10 @@
         <v>11</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>14</v>
@@ -2261,7 +2264,7 @@
         <v>45647</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2272,10 +2275,10 @@
         <v>11</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>14</v>
@@ -2293,7 +2296,7 @@
         <v>45739</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2304,10 +2307,10 @@
         <v>11</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>14</v>
@@ -2325,7 +2328,7 @@
         <v>45634</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2336,10 +2339,10 @@
         <v>11</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>14</v>
@@ -2357,7 +2360,7 @@
         <v>45714</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2368,10 +2371,10 @@
         <v>11</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>14</v>
@@ -2389,7 +2392,7 @@
         <v>45601</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2400,7 +2403,7 @@
         <v>11</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>13</v>
@@ -2421,7 +2424,7 @@
         <v>45541</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,10 +2435,10 @@
         <v>11</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>14</v>
@@ -2453,7 +2456,7 @@
         <v>45658</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2464,10 +2467,10 @@
         <v>11</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>14</v>
@@ -2485,7 +2488,7 @@
         <v>45617</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,10 +2499,10 @@
         <v>11</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>14</v>
@@ -2517,7 +2520,7 @@
         <v>45641</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2528,10 +2531,10 @@
         <v>11</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>14</v>
@@ -2549,7 +2552,7 @@
         <v>45507</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2560,10 +2563,10 @@
         <v>11</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>14</v>
@@ -2581,7 +2584,7 @@
         <v>45581</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2592,10 +2595,10 @@
         <v>11</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>14</v>
@@ -2613,7 +2616,7 @@
         <v>45580</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2624,10 +2627,10 @@
         <v>11</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>14</v>
@@ -2645,7 +2648,7 @@
         <v>45676</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2656,10 +2659,10 @@
         <v>11</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E42" s="0" t="s">
         <v>14</v>
@@ -2677,7 +2680,7 @@
         <v>45666</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2688,7 +2691,7 @@
         <v>11</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>13</v>
@@ -2709,7 +2712,7 @@
         <v>45656</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2720,10 +2723,10 @@
         <v>11</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E44" s="0" t="s">
         <v>14</v>
@@ -2741,7 +2744,7 @@
         <v>45693</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2752,7 +2755,7 @@
         <v>11</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>13</v>
@@ -2773,7 +2776,7 @@
         <v>45682</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2784,10 +2787,10 @@
         <v>11</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E46" s="0" t="s">
         <v>14</v>
@@ -2805,7 +2808,7 @@
         <v>45628</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2816,10 +2819,10 @@
         <v>11</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E47" s="0" t="s">
         <v>14</v>
@@ -2837,7 +2840,7 @@
         <v>45738</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2848,7 +2851,7 @@
         <v>11</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>13</v>
@@ -2869,7 +2872,7 @@
         <v>45490</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2880,7 +2883,7 @@
         <v>11</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>13</v>
@@ -2901,7 +2904,7 @@
         <v>45692</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2912,7 +2915,7 @@
         <v>11</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>13</v>
@@ -2933,7 +2936,7 @@
         <v>45728</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2944,7 +2947,7 @@
         <v>11</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>13</v>
@@ -2965,7 +2968,7 @@
         <v>45737</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2976,7 +2979,7 @@
         <v>11</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>13</v>
@@ -2997,7 +3000,7 @@
         <v>45666</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3008,7 +3011,7 @@
         <v>11</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>13</v>
@@ -3029,7 +3032,7 @@
         <v>45744</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3040,7 +3043,7 @@
         <v>11</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>13</v>
@@ -3061,7 +3064,7 @@
         <v>45579</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3072,7 +3075,7 @@
         <v>11</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>13</v>
@@ -3093,7 +3096,7 @@
         <v>45495</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3104,7 +3107,7 @@
         <v>11</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>13</v>
@@ -3125,7 +3128,7 @@
         <v>45726</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3136,7 +3139,7 @@
         <v>11</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>13</v>
@@ -3157,7 +3160,7 @@
         <v>45602</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3168,7 +3171,7 @@
         <v>11</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>13</v>
@@ -3189,7 +3192,7 @@
         <v>45486</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3200,7 +3203,7 @@
         <v>11</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>13</v>
@@ -3221,7 +3224,7 @@
         <v>45609</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3232,7 +3235,7 @@
         <v>11</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>13</v>
@@ -3253,7 +3256,7 @@
         <v>45524</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3264,7 +3267,7 @@
         <v>11</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>13</v>
@@ -3285,7 +3288,7 @@
         <v>45745</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3296,7 +3299,7 @@
         <v>11</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>13</v>
@@ -3317,7 +3320,7 @@
         <v>45596</v>
       </c>
       <c r="J62" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3328,7 +3331,7 @@
         <v>11</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>13</v>
@@ -3349,7 +3352,7 @@
         <v>45604</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3360,7 +3363,7 @@
         <v>11</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>13</v>
@@ -3381,7 +3384,7 @@
         <v>45704</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3392,7 +3395,7 @@
         <v>11</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>13</v>
@@ -3413,7 +3416,7 @@
         <v>45554</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3424,7 +3427,7 @@
         <v>11</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>13</v>
@@ -3445,7 +3448,7 @@
         <v>45573</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3456,7 +3459,7 @@
         <v>11</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>13</v>
@@ -3477,7 +3480,7 @@
         <v>45729</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3488,7 +3491,7 @@
         <v>11</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>13</v>
@@ -3509,7 +3512,7 @@
         <v>45611</v>
       </c>
       <c r="J68" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3520,7 +3523,7 @@
         <v>11</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>13</v>
@@ -3541,7 +3544,7 @@
         <v>45731</v>
       </c>
       <c r="J69" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3552,7 +3555,7 @@
         <v>11</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>13</v>
@@ -3573,7 +3576,7 @@
         <v>45487</v>
       </c>
       <c r="J70" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3584,7 +3587,7 @@
         <v>11</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>13</v>
@@ -3605,7 +3608,7 @@
         <v>45546</v>
       </c>
       <c r="J71" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3616,7 +3619,7 @@
         <v>11</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>13</v>
@@ -3637,7 +3640,7 @@
         <v>45578</v>
       </c>
       <c r="J72" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3648,7 +3651,7 @@
         <v>11</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>13</v>
@@ -3669,7 +3672,7 @@
         <v>45696</v>
       </c>
       <c r="J73" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3680,7 +3683,7 @@
         <v>11</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D74" s="0" t="s">
         <v>13</v>
@@ -3701,7 +3704,7 @@
         <v>45528</v>
       </c>
       <c r="J74" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3712,7 +3715,7 @@
         <v>11</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>13</v>
@@ -3733,7 +3736,7 @@
         <v>45574</v>
       </c>
       <c r="J75" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3744,7 +3747,7 @@
         <v>11</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D76" s="0" t="s">
         <v>13</v>
@@ -3765,7 +3768,7 @@
         <v>45583</v>
       </c>
       <c r="J76" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3776,10 +3779,10 @@
         <v>11</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E77" s="0" t="s">
         <v>14</v>
@@ -3797,7 +3800,7 @@
         <v>45566</v>
       </c>
       <c r="J77" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3808,10 +3811,10 @@
         <v>11</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E78" s="0" t="s">
         <v>14</v>
@@ -3829,7 +3832,7 @@
         <v>45682</v>
       </c>
       <c r="J78" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3840,10 +3843,10 @@
         <v>11</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E79" s="0" t="s">
         <v>14</v>
@@ -3861,7 +3864,7 @@
         <v>45737</v>
       </c>
       <c r="J79" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3872,10 +3875,10 @@
         <v>11</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E80" s="0" t="s">
         <v>14</v>
@@ -3893,7 +3896,7 @@
         <v>45525</v>
       </c>
       <c r="J80" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3904,10 +3907,10 @@
         <v>11</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E81" s="0" t="s">
         <v>14</v>
@@ -3925,7 +3928,7 @@
         <v>45712</v>
       </c>
       <c r="J81" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3936,10 +3939,10 @@
         <v>11</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E82" s="0" t="s">
         <v>14</v>
@@ -3957,7 +3960,7 @@
         <v>45612</v>
       </c>
       <c r="J82" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3968,10 +3971,10 @@
         <v>11</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E83" s="0" t="s">
         <v>14</v>
@@ -3989,7 +3992,7 @@
         <v>45740</v>
       </c>
       <c r="J83" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4000,10 +4003,10 @@
         <v>11</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E84" s="0" t="s">
         <v>14</v>
@@ -4021,7 +4024,7 @@
         <v>45669</v>
       </c>
       <c r="J84" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4032,7 +4035,7 @@
         <v>11</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D85" s="0" t="s">
         <v>13</v>
@@ -4053,7 +4056,7 @@
         <v>45736</v>
       </c>
       <c r="J85" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4064,7 +4067,7 @@
         <v>11</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D86" s="0" t="s">
         <v>13</v>
@@ -4085,7 +4088,7 @@
         <v>45667</v>
       </c>
       <c r="J86" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4096,7 +4099,7 @@
         <v>11</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D87" s="0" t="s">
         <v>13</v>
@@ -4117,7 +4120,7 @@
         <v>45641</v>
       </c>
       <c r="J87" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4128,10 +4131,10 @@
         <v>11</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E88" s="0" t="s">
         <v>14</v>
@@ -4149,7 +4152,7 @@
         <v>45513</v>
       </c>
       <c r="J88" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4160,10 +4163,10 @@
         <v>11</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E89" s="0" t="s">
         <v>14</v>
@@ -4181,7 +4184,7 @@
         <v>45586</v>
       </c>
       <c r="J89" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4192,10 +4195,10 @@
         <v>11</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E90" s="0" t="s">
         <v>14</v>
@@ -4213,7 +4216,7 @@
         <v>45661</v>
       </c>
       <c r="J90" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4224,10 +4227,10 @@
         <v>11</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E91" s="0" t="s">
         <v>14</v>
@@ -4245,7 +4248,7 @@
         <v>45696</v>
       </c>
       <c r="J91" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4256,7 +4259,7 @@
         <v>11</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D92" s="0" t="s">
         <v>13</v>
@@ -4277,7 +4280,7 @@
         <v>45553</v>
       </c>
       <c r="J92" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4288,10 +4291,10 @@
         <v>11</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E93" s="0" t="s">
         <v>14</v>
@@ -4309,7 +4312,7 @@
         <v>45557</v>
       </c>
       <c r="J93" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4320,10 +4323,10 @@
         <v>11</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E94" s="0" t="s">
         <v>14</v>
@@ -4341,7 +4344,7 @@
         <v>45559</v>
       </c>
       <c r="J94" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4352,10 +4355,10 @@
         <v>11</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E95" s="0" t="s">
         <v>14</v>
@@ -4373,7 +4376,7 @@
         <v>45590</v>
       </c>
       <c r="J95" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4384,7 +4387,7 @@
         <v>11</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D96" s="0" t="s">
         <v>13</v>
@@ -4405,7 +4408,7 @@
         <v>45509</v>
       </c>
       <c r="J96" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4416,10 +4419,10 @@
         <v>11</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E97" s="0" t="s">
         <v>14</v>
@@ -4437,7 +4440,7 @@
         <v>45637</v>
       </c>
       <c r="J97" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4448,10 +4451,10 @@
         <v>11</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E98" s="0" t="s">
         <v>14</v>
@@ -4469,7 +4472,7 @@
         <v>45687</v>
       </c>
       <c r="J98" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4480,10 +4483,10 @@
         <v>11</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E99" s="0" t="s">
         <v>14</v>
@@ -4501,7 +4504,7 @@
         <v>45513</v>
       </c>
       <c r="J99" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4512,10 +4515,10 @@
         <v>11</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E100" s="0" t="s">
         <v>14</v>
@@ -4533,7 +4536,7 @@
         <v>45693</v>
       </c>
       <c r="J100" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4544,10 +4547,10 @@
         <v>11</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E101" s="0" t="s">
         <v>14</v>
@@ -4565,7 +4568,7 @@
         <v>45479</v>
       </c>
       <c r="J101" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4576,10 +4579,10 @@
         <v>11</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E102" s="0" t="s">
         <v>14</v>
@@ -4597,7 +4600,7 @@
         <v>45651</v>
       </c>
       <c r="J102" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4608,10 +4611,10 @@
         <v>11</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E103" s="0" t="s">
         <v>14</v>
@@ -4629,7 +4632,7 @@
         <v>45637</v>
       </c>
       <c r="J103" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4640,10 +4643,10 @@
         <v>11</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E104" s="0" t="s">
         <v>14</v>
@@ -4661,7 +4664,7 @@
         <v>45679</v>
       </c>
       <c r="J104" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4672,7 +4675,7 @@
         <v>11</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D105" s="0" t="s">
         <v>13</v>
@@ -4693,7 +4696,7 @@
         <v>45687</v>
       </c>
       <c r="J105" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4704,10 +4707,10 @@
         <v>11</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E106" s="0" t="s">
         <v>14</v>
@@ -4725,7 +4728,7 @@
         <v>45699</v>
       </c>
       <c r="J106" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4736,10 +4739,10 @@
         <v>11</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E107" s="0" t="s">
         <v>14</v>
@@ -4757,7 +4760,7 @@
         <v>45596</v>
       </c>
       <c r="J107" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4768,10 +4771,10 @@
         <v>11</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E108" s="0" t="s">
         <v>14</v>
@@ -4789,7 +4792,7 @@
         <v>45659</v>
       </c>
       <c r="J108" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4800,10 +4803,10 @@
         <v>11</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E109" s="0" t="s">
         <v>14</v>
@@ -4821,7 +4824,7 @@
         <v>45614</v>
       </c>
       <c r="J109" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4832,7 +4835,7 @@
         <v>11</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D110" s="0" t="s">
         <v>13</v>
@@ -4853,7 +4856,7 @@
         <v>45510</v>
       </c>
       <c r="J110" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4864,7 +4867,7 @@
         <v>11</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D111" s="0" t="s">
         <v>13</v>
@@ -4885,7 +4888,7 @@
         <v>45534</v>
       </c>
       <c r="J111" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4896,10 +4899,10 @@
         <v>11</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E112" s="0" t="s">
         <v>14</v>
@@ -4917,7 +4920,7 @@
         <v>45489</v>
       </c>
       <c r="J112" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4928,10 +4931,10 @@
         <v>11</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E113" s="0" t="s">
         <v>14</v>
@@ -4949,7 +4952,7 @@
         <v>45582</v>
       </c>
       <c r="J113" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4960,10 +4963,10 @@
         <v>11</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E114" s="0" t="s">
         <v>14</v>
@@ -4981,7 +4984,7 @@
         <v>45695</v>
       </c>
       <c r="J114" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4992,7 +4995,7 @@
         <v>11</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D115" s="0" t="s">
         <v>13</v>
@@ -5013,7 +5016,7 @@
         <v>45551</v>
       </c>
       <c r="J115" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5024,10 +5027,10 @@
         <v>11</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E116" s="0" t="s">
         <v>14</v>
@@ -5045,7 +5048,7 @@
         <v>45539</v>
       </c>
       <c r="J116" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5056,10 +5059,10 @@
         <v>11</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E117" s="0" t="s">
         <v>14</v>
@@ -5077,7 +5080,7 @@
         <v>45656</v>
       </c>
       <c r="J117" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5088,10 +5091,10 @@
         <v>11</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E118" s="0" t="s">
         <v>14</v>
@@ -5109,7 +5112,7 @@
         <v>45505</v>
       </c>
       <c r="J118" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5120,10 +5123,10 @@
         <v>11</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E119" s="0" t="s">
         <v>14</v>
@@ -5141,7 +5144,7 @@
         <v>45721</v>
       </c>
       <c r="J119" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5152,10 +5155,10 @@
         <v>11</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E120" s="0" t="s">
         <v>14</v>
@@ -5173,7 +5176,7 @@
         <v>45581</v>
       </c>
       <c r="J120" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5184,7 +5187,7 @@
         <v>11</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D121" s="0" t="s">
         <v>13</v>
@@ -5205,7 +5208,7 @@
         <v>45648</v>
       </c>
       <c r="J121" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5216,10 +5219,10 @@
         <v>11</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E122" s="0" t="s">
         <v>14</v>
@@ -5237,7 +5240,7 @@
         <v>45661</v>
       </c>
       <c r="J122" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5248,10 +5251,10 @@
         <v>11</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E123" s="0" t="s">
         <v>14</v>
@@ -5269,7 +5272,7 @@
         <v>45706</v>
       </c>
       <c r="J123" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5280,10 +5283,10 @@
         <v>11</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E124" s="0" t="s">
         <v>14</v>
@@ -5301,7 +5304,7 @@
         <v>45615</v>
       </c>
       <c r="J124" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5312,10 +5315,10 @@
         <v>11</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E125" s="0" t="s">
         <v>14</v>
@@ -5333,7 +5336,7 @@
         <v>45720</v>
       </c>
       <c r="J125" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5344,10 +5347,10 @@
         <v>11</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E126" s="0" t="s">
         <v>14</v>
@@ -5365,7 +5368,7 @@
         <v>45659</v>
       </c>
       <c r="J126" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5376,10 +5379,10 @@
         <v>11</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E127" s="0" t="s">
         <v>14</v>
@@ -5397,7 +5400,7 @@
         <v>45477</v>
       </c>
       <c r="J127" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5408,10 +5411,10 @@
         <v>11</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E128" s="0" t="s">
         <v>14</v>
@@ -5429,7 +5432,7 @@
         <v>45529</v>
       </c>
       <c r="J128" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5440,10 +5443,10 @@
         <v>11</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E129" s="0" t="s">
         <v>14</v>
@@ -5461,7 +5464,7 @@
         <v>45566</v>
       </c>
       <c r="J129" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5472,10 +5475,10 @@
         <v>11</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E130" s="0" t="s">
         <v>14</v>
@@ -5493,7 +5496,7 @@
         <v>45595</v>
       </c>
       <c r="J130" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5504,10 +5507,10 @@
         <v>11</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E131" s="0" t="s">
         <v>14</v>
@@ -5525,7 +5528,7 @@
         <v>45643</v>
       </c>
       <c r="J131" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5536,10 +5539,10 @@
         <v>11</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E132" s="0" t="s">
         <v>14</v>
@@ -5557,7 +5560,7 @@
         <v>45701</v>
       </c>
       <c r="J132" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5568,10 +5571,10 @@
         <v>11</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E133" s="0" t="s">
         <v>14</v>
@@ -5589,7 +5592,7 @@
         <v>45695</v>
       </c>
       <c r="J133" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5600,10 +5603,10 @@
         <v>11</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E134" s="0" t="s">
         <v>14</v>
@@ -5621,7 +5624,7 @@
         <v>45573</v>
       </c>
       <c r="J134" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5632,10 +5635,10 @@
         <v>11</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E135" s="0" t="s">
         <v>14</v>
@@ -5653,7 +5656,7 @@
         <v>45491</v>
       </c>
       <c r="J135" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5664,10 +5667,10 @@
         <v>11</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E136" s="0" t="s">
         <v>14</v>
@@ -5685,7 +5688,7 @@
         <v>45724</v>
       </c>
       <c r="J136" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5696,10 +5699,10 @@
         <v>11</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D137" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E137" s="0" t="s">
         <v>14</v>
@@ -5717,7 +5720,7 @@
         <v>45702</v>
       </c>
       <c r="J137" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5728,10 +5731,10 @@
         <v>11</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D138" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E138" s="0" t="s">
         <v>14</v>
@@ -5749,7 +5752,7 @@
         <v>45564</v>
       </c>
       <c r="J138" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5760,10 +5763,10 @@
         <v>11</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D139" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E139" s="0" t="s">
         <v>14</v>
@@ -5781,7 +5784,7 @@
         <v>45740</v>
       </c>
       <c r="J139" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5792,10 +5795,10 @@
         <v>11</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D140" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E140" s="0" t="s">
         <v>14</v>
@@ -5813,7 +5816,7 @@
         <v>45739</v>
       </c>
       <c r="J140" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5824,7 +5827,7 @@
         <v>11</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D141" s="0" t="s">
         <v>13</v>
@@ -5845,7 +5848,7 @@
         <v>45537</v>
       </c>
       <c r="J141" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5856,7 +5859,7 @@
         <v>11</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D142" s="0" t="s">
         <v>13</v>
@@ -5877,7 +5880,7 @@
         <v>45644</v>
       </c>
       <c r="J142" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5888,13 +5891,13 @@
         <v>11</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E143" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F143" s="0" t="n">
         <v>922502</v>
@@ -5909,7 +5912,7 @@
         <v>45558</v>
       </c>
       <c r="J143" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5920,13 +5923,13 @@
         <v>11</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E144" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F144" s="0" t="n">
         <v>107479977958</v>
@@ -5941,7 +5944,7 @@
         <v>45558</v>
       </c>
       <c r="J144" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5952,13 +5955,13 @@
         <v>11</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D145" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E145" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F145" s="0" t="n">
         <v>1513110595</v>
@@ -5973,7 +5976,7 @@
         <v>45512</v>
       </c>
       <c r="J145" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5984,13 +5987,13 @@
         <v>11</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D146" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E146" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F146" s="0" t="n">
         <v>3191171</v>
@@ -6005,7 +6008,7 @@
         <v>45561</v>
       </c>
       <c r="J146" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6016,13 +6019,13 @@
         <v>11</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D147" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E147" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F147" s="0" t="n">
         <v>62817229110</v>
@@ -6037,7 +6040,7 @@
         <v>45606</v>
       </c>
       <c r="J147" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6048,13 +6051,13 @@
         <v>11</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D148" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E148" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F148" s="0" t="n">
         <v>7564700178</v>
@@ -6069,7 +6072,7 @@
         <v>45504</v>
       </c>
       <c r="J148" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6080,13 +6083,13 @@
         <v>11</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D149" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E149" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F149" s="0" t="n">
         <v>39315055</v>
@@ -6101,7 +6104,7 @@
         <v>45515</v>
       </c>
       <c r="J149" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6112,13 +6115,13 @@
         <v>11</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D150" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E150" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F150" s="0" t="n">
         <v>806341</v>
@@ -6133,7 +6136,7 @@
         <v>45483</v>
       </c>
       <c r="J150" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6144,13 +6147,13 @@
         <v>11</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D151" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E151" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F151" s="0" t="n">
         <v>33220182</v>
@@ -6165,7 +6168,7 @@
         <v>45529</v>
       </c>
       <c r="J151" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6176,13 +6179,13 @@
         <v>11</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D152" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E152" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F152" s="0" t="n">
         <v>8660373851</v>
@@ -6197,7 +6200,7 @@
         <v>45576</v>
       </c>
       <c r="J152" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6208,13 +6211,13 @@
         <v>11</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D153" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E153" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F153" s="0" t="n">
         <v>7173269088</v>
@@ -6229,7 +6232,7 @@
         <v>45708</v>
       </c>
       <c r="J153" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6240,13 +6243,13 @@
         <v>11</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D154" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E154" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F154" s="0" t="n">
         <v>76767069</v>
@@ -6261,7 +6264,7 @@
         <v>45563</v>
       </c>
       <c r="J154" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6272,13 +6275,13 @@
         <v>11</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D155" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E155" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F155" s="0" t="n">
         <v>564985</v>
@@ -6293,7 +6296,7 @@
         <v>45661</v>
       </c>
       <c r="J155" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6304,13 +6307,13 @@
         <v>11</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D156" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E156" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F156" s="0" t="n">
         <v>113017787401</v>
@@ -6325,7 +6328,7 @@
         <v>45519</v>
       </c>
       <c r="J156" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6336,13 +6339,13 @@
         <v>11</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D157" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E157" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F157" s="0" t="n">
         <v>6479530310</v>
@@ -6357,7 +6360,7 @@
         <v>45507</v>
       </c>
       <c r="J157" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6368,13 +6371,13 @@
         <v>11</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D158" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E158" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F158" s="0" t="n">
         <v>787374</v>
@@ -6389,7 +6392,7 @@
         <v>45690</v>
       </c>
       <c r="J158" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6400,13 +6403,13 @@
         <v>11</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D159" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E159" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F159" s="0" t="n">
         <v>626885167170</v>
@@ -6421,7 +6424,7 @@
         <v>45532</v>
       </c>
       <c r="J159" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6432,13 +6435,13 @@
         <v>11</v>
       </c>
       <c r="C160" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D160" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E160" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F160" s="0" t="n">
         <v>87073583</v>
@@ -6453,7 +6456,7 @@
         <v>45484</v>
       </c>
       <c r="J160" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6464,13 +6467,13 @@
         <v>11</v>
       </c>
       <c r="C161" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D161" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E161" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F161" s="0" t="n">
         <v>676472</v>
@@ -6485,7 +6488,7 @@
         <v>45681</v>
       </c>
       <c r="J161" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6496,7 +6499,7 @@
         <v>11</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D162" s="0" t="s">
         <v>13</v>
@@ -6517,7 +6520,7 @@
         <v>45540</v>
       </c>
       <c r="J162" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6528,7 +6531,7 @@
         <v>11</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D163" s="0" t="s">
         <v>13</v>
@@ -6549,7 +6552,7 @@
         <v>45644</v>
       </c>
       <c r="J163" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6560,10 +6563,10 @@
         <v>11</v>
       </c>
       <c r="C164" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D164" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E164" s="0" t="s">
         <v>14</v>
@@ -6581,7 +6584,7 @@
         <v>45617</v>
       </c>
       <c r="J164" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6592,10 +6595,10 @@
         <v>11</v>
       </c>
       <c r="C165" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D165" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E165" s="0" t="s">
         <v>14</v>
@@ -6613,7 +6616,7 @@
         <v>45674</v>
       </c>
       <c r="J165" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6624,10 +6627,10 @@
         <v>11</v>
       </c>
       <c r="C166" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D166" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E166" s="0" t="s">
         <v>14</v>
@@ -6645,7 +6648,7 @@
         <v>45479</v>
       </c>
       <c r="J166" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6656,10 +6659,10 @@
         <v>11</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D167" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E167" s="0" t="s">
         <v>14</v>
@@ -6677,7 +6680,7 @@
         <v>45515</v>
       </c>
       <c r="J167" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6688,10 +6691,10 @@
         <v>11</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E168" s="0" t="s">
         <v>14</v>
@@ -6709,7 +6712,7 @@
         <v>45634</v>
       </c>
       <c r="J168" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6720,10 +6723,10 @@
         <v>11</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D169" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E169" s="0" t="s">
         <v>14</v>
@@ -6741,7 +6744,7 @@
         <v>45504</v>
       </c>
       <c r="J169" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6752,7 +6755,7 @@
         <v>11</v>
       </c>
       <c r="C170" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D170" s="0" t="s">
         <v>13</v>
@@ -6773,7 +6776,7 @@
         <v>45537</v>
       </c>
       <c r="J170" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6784,10 +6787,10 @@
         <v>11</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D171" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E171" s="0" t="s">
         <v>14</v>
@@ -6805,7 +6808,7 @@
         <v>45527</v>
       </c>
       <c r="J171" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6816,13 +6819,13 @@
         <v>11</v>
       </c>
       <c r="C172" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D172" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E172" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F172" s="0" t="n">
         <v>206264</v>
@@ -6837,7 +6840,7 @@
         <v>45735</v>
       </c>
       <c r="J172" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6848,13 +6851,13 @@
         <v>11</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D173" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E173" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F173" s="0" t="n">
         <v>48066811343</v>
@@ -6869,7 +6872,7 @@
         <v>45658</v>
       </c>
       <c r="J173" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6880,13 +6883,13 @@
         <v>11</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D174" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E174" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F174" s="0" t="n">
         <v>261476</v>
@@ -6901,7 +6904,7 @@
         <v>45480</v>
       </c>
       <c r="J174" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6912,13 +6915,13 @@
         <v>11</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D175" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E175" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F175" s="0" t="n">
         <v>311663704102</v>
@@ -6933,7 +6936,7 @@
         <v>45565</v>
       </c>
       <c r="J175" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6944,13 +6947,13 @@
         <v>11</v>
       </c>
       <c r="C176" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D176" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E176" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F176" s="0" t="n">
         <v>99085273</v>
@@ -6965,7 +6968,7 @@
         <v>45736</v>
       </c>
       <c r="J176" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6976,13 +6979,13 @@
         <v>11</v>
       </c>
       <c r="C177" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D177" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E177" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F177" s="0" t="n">
         <v>491810095347</v>
@@ -6997,7 +7000,7 @@
         <v>45703</v>
       </c>
       <c r="J177" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7008,13 +7011,13 @@
         <v>11</v>
       </c>
       <c r="C178" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D178" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E178" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F178" s="0" t="n">
         <v>9595284085</v>
@@ -7029,7 +7032,7 @@
         <v>45538</v>
       </c>
       <c r="J178" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7040,13 +7043,13 @@
         <v>11</v>
       </c>
       <c r="C179" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D179" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E179" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F179" s="0" t="n">
         <v>7285382952</v>
@@ -7061,7 +7064,7 @@
         <v>45563</v>
       </c>
       <c r="J179" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7072,13 +7075,13 @@
         <v>11</v>
       </c>
       <c r="C180" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D180" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E180" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F180" s="0" t="n">
         <v>483072700</v>
@@ -7093,7 +7096,7 @@
         <v>45622</v>
       </c>
       <c r="J180" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7104,13 +7107,13 @@
         <v>11</v>
       </c>
       <c r="C181" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D181" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E181" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F181" s="0" t="n">
         <v>951047385</v>
@@ -7125,7 +7128,7 @@
         <v>45601</v>
       </c>
       <c r="J181" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7136,13 +7139,13 @@
         <v>11</v>
       </c>
       <c r="C182" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="D182" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E182" s="0" t="s">
         <v>312</v>
-      </c>
-      <c r="D182" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E182" s="0" t="s">
-        <v>311</v>
       </c>
       <c r="F182" s="0" t="n">
         <v>5188981652</v>
@@ -7168,13 +7171,13 @@
         <v>11</v>
       </c>
       <c r="C183" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D183" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E183" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F183" s="0" t="n">
         <v>8830053804</v>
@@ -7200,7 +7203,7 @@
         <v>11</v>
       </c>
       <c r="C184" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D184" s="0" t="s">
         <v>13</v>
@@ -7221,7 +7224,7 @@
         <v>45581</v>
       </c>
       <c r="J184" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7232,10 +7235,10 @@
         <v>11</v>
       </c>
       <c r="C185" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D185" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E185" s="0" t="s">
         <v>14</v>
@@ -7253,7 +7256,7 @@
         <v>45655</v>
       </c>
       <c r="J185" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7264,7 +7267,7 @@
         <v>11</v>
       </c>
       <c r="C186" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D186" s="0" t="s">
         <v>13</v>
@@ -7285,7 +7288,7 @@
         <v>45697</v>
       </c>
       <c r="J186" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7296,13 +7299,13 @@
         <v>11</v>
       </c>
       <c r="C187" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D187" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E187" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F187" s="0" t="n">
         <v>727659058994</v>
@@ -7317,7 +7320,7 @@
         <v>45573</v>
       </c>
       <c r="J187" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7328,13 +7331,13 @@
         <v>11</v>
       </c>
       <c r="C188" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D188" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E188" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F188" s="0" t="n">
         <v>6041531</v>
@@ -7349,7 +7352,7 @@
         <v>45690</v>
       </c>
       <c r="J188" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7360,13 +7363,13 @@
         <v>11</v>
       </c>
       <c r="C189" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D189" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E189" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F189" s="0" t="n">
         <v>8839610860</v>
@@ -7381,7 +7384,7 @@
         <v>45487</v>
       </c>
       <c r="J189" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7392,13 +7395,13 @@
         <v>11</v>
       </c>
       <c r="C190" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D190" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E190" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F190" s="0" t="n">
         <v>10331653</v>
@@ -7413,7 +7416,7 @@
         <v>45634</v>
       </c>
       <c r="J190" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7424,10 +7427,10 @@
         <v>11</v>
       </c>
       <c r="C191" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D191" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E191" s="0" t="s">
         <v>14</v>
@@ -7445,7 +7448,7 @@
         <v>45743</v>
       </c>
       <c r="J191" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7456,10 +7459,10 @@
         <v>11</v>
       </c>
       <c r="C192" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D192" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E192" s="0" t="s">
         <v>14</v>
@@ -7477,7 +7480,7 @@
         <v>45539</v>
       </c>
       <c r="J192" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7488,13 +7491,13 @@
         <v>11</v>
       </c>
       <c r="C193" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D193" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E193" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F193" s="0" t="n">
         <v>3011024</v>
@@ -7509,7 +7512,7 @@
         <v>45710</v>
       </c>
       <c r="J193" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7520,10 +7523,10 @@
         <v>11</v>
       </c>
       <c r="C194" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D194" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E194" s="0" t="s">
         <v>14</v>
@@ -7541,7 +7544,7 @@
         <v>45589</v>
       </c>
       <c r="J194" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7552,10 +7555,10 @@
         <v>11</v>
       </c>
       <c r="C195" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D195" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E195" s="0" t="s">
         <v>14</v>
@@ -7573,7 +7576,7 @@
         <v>45648</v>
       </c>
       <c r="J195" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7584,10 +7587,10 @@
         <v>11</v>
       </c>
       <c r="C196" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D196" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E196" s="0" t="s">
         <v>14</v>
@@ -7605,7 +7608,7 @@
         <v>45557</v>
       </c>
       <c r="J196" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7616,10 +7619,10 @@
         <v>11</v>
       </c>
       <c r="C197" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D197" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E197" s="0" t="s">
         <v>14</v>
@@ -7637,7 +7640,7 @@
         <v>45665</v>
       </c>
       <c r="J197" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7648,7 +7651,7 @@
         <v>11</v>
       </c>
       <c r="C198" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D198" s="0" t="s">
         <v>13</v>
@@ -7669,7 +7672,7 @@
         <v>45518</v>
       </c>
       <c r="J198" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7680,7 +7683,7 @@
         <v>11</v>
       </c>
       <c r="C199" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D199" s="0" t="s">
         <v>13</v>
@@ -7701,7 +7704,7 @@
         <v>45539</v>
       </c>
       <c r="J199" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7712,10 +7715,10 @@
         <v>11</v>
       </c>
       <c r="C200" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D200" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E200" s="0" t="s">
         <v>14</v>
@@ -7733,7 +7736,7 @@
         <v>45547</v>
       </c>
       <c r="J200" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7744,13 +7747,13 @@
         <v>11</v>
       </c>
       <c r="C201" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D201" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E201" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F201" s="0" t="n">
         <v>79255121323</v>
@@ -7759,7 +7762,7 @@
         <v>1</v>
       </c>
       <c r="H201" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="I201" s="2" t="n">
         <v>45559</v>
@@ -7773,13 +7776,13 @@
         <v>11</v>
       </c>
       <c r="C202" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D202" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E202" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F202" s="0" t="n">
         <v>1405157491</v>
@@ -7794,7 +7797,7 @@
         <v>45696</v>
       </c>
       <c r="J202" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7805,13 +7808,13 @@
         <v>11</v>
       </c>
       <c r="C203" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D203" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E203" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F203" s="0" t="n">
         <v>6984951</v>
@@ -7826,7 +7829,7 @@
         <v>45483</v>
       </c>
       <c r="J203" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7837,13 +7840,13 @@
         <v>11</v>
       </c>
       <c r="C204" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D204" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E204" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F204" s="0" t="n">
         <v>129489134167</v>
@@ -7858,7 +7861,7 @@
         <v>45646</v>
       </c>
       <c r="J204" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7869,13 +7872,13 @@
         <v>11</v>
       </c>
       <c r="C205" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D205" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E205" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F205" s="0" t="n">
         <v>29684373</v>
@@ -7890,7 +7893,7 @@
         <v>45546</v>
       </c>
       <c r="J205" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7901,13 +7904,13 @@
         <v>11</v>
       </c>
       <c r="C206" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D206" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E206" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F206" s="0" t="n">
         <v>25334895</v>
@@ -7922,7 +7925,7 @@
         <v>45522</v>
       </c>
       <c r="J206" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7933,13 +7936,13 @@
         <v>11</v>
       </c>
       <c r="C207" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D207" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E207" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F207" s="0" t="n">
         <v>8196549819</v>
@@ -7954,7 +7957,7 @@
         <v>45620</v>
       </c>
       <c r="J207" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7965,13 +7968,13 @@
         <v>11</v>
       </c>
       <c r="C208" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D208" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E208" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F208" s="0" t="n">
         <v>186691</v>
@@ -7986,7 +7989,7 @@
         <v>45696</v>
       </c>
       <c r="J208" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7997,13 +8000,13 @@
         <v>11</v>
       </c>
       <c r="C209" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D209" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E209" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F209" s="0" t="n">
         <v>124839445</v>
@@ -8018,7 +8021,7 @@
         <v>45575</v>
       </c>
       <c r="J209" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8029,13 +8032,13 @@
         <v>11</v>
       </c>
       <c r="C210" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D210" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E210" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F210" s="0" t="n">
         <v>589260457</v>
@@ -8050,7 +8053,7 @@
         <v>45671</v>
       </c>
       <c r="J210" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8061,13 +8064,13 @@
         <v>11</v>
       </c>
       <c r="C211" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D211" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E211" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F211" s="0" t="n">
         <v>941190417</v>
@@ -8082,7 +8085,7 @@
         <v>45618</v>
       </c>
       <c r="J211" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8093,13 +8096,13 @@
         <v>11</v>
       </c>
       <c r="C212" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D212" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E212" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F212" s="0" t="n">
         <v>5490867279</v>
@@ -8114,7 +8117,7 @@
         <v>45609</v>
       </c>
       <c r="J212" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8125,13 +8128,13 @@
         <v>11</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D213" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E213" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F213" s="0" t="n">
         <v>73678013427</v>
@@ -8146,7 +8149,7 @@
         <v>45512</v>
       </c>
       <c r="J213" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8157,13 +8160,13 @@
         <v>11</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D214" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E214" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F214" s="0" t="n">
         <v>6023391</v>
@@ -8178,7 +8181,7 @@
         <v>45600</v>
       </c>
       <c r="J214" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8189,13 +8192,13 @@
         <v>11</v>
       </c>
       <c r="C215" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D215" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E215" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F215" s="0" t="n">
         <v>598867</v>
@@ -8221,13 +8224,13 @@
         <v>11</v>
       </c>
       <c r="C216" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D216" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E216" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="F216" s="0" t="n">
         <v>34414881476</v>
@@ -8242,7 +8245,7 @@
         <v>45661</v>
       </c>
       <c r="J216" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8253,13 +8256,13 @@
         <v>11</v>
       </c>
       <c r="C217" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D217" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E217" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="F217" s="0" t="n">
         <v>428516229</v>
@@ -8274,7 +8277,7 @@
         <v>45621</v>
       </c>
       <c r="J217" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8285,13 +8288,13 @@
         <v>11</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D218" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E218" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F218" s="0" t="n">
         <v>140961878479</v>
@@ -8306,7 +8309,7 @@
         <v>45727</v>
       </c>
       <c r="J218" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8317,13 +8320,13 @@
         <v>11</v>
       </c>
       <c r="C219" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D219" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E219" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F219" s="0" t="n">
         <v>92285640672</v>
@@ -8338,7 +8341,7 @@
         <v>45642</v>
       </c>
       <c r="J219" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8349,10 +8352,10 @@
         <v>11</v>
       </c>
       <c r="C220" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D220" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E220" s="0" t="s">
         <v>14</v>
@@ -8370,7 +8373,7 @@
         <v>45503</v>
       </c>
       <c r="J220" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8381,10 +8384,10 @@
         <v>11</v>
       </c>
       <c r="C221" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D221" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E221" s="0" t="s">
         <v>14</v>
@@ -8402,7 +8405,7 @@
         <v>45586</v>
       </c>
       <c r="J221" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8413,10 +8416,10 @@
         <v>11</v>
       </c>
       <c r="C222" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D222" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E222" s="0" t="s">
         <v>14</v>
@@ -8434,7 +8437,7 @@
         <v>45479</v>
       </c>
       <c r="J222" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8445,10 +8448,10 @@
         <v>11</v>
       </c>
       <c r="C223" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D223" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E223" s="0" t="s">
         <v>14</v>
@@ -8466,7 +8469,7 @@
         <v>45722</v>
       </c>
       <c r="J223" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8477,13 +8480,13 @@
         <v>11</v>
       </c>
       <c r="C224" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D224" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E224" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F224" s="0" t="n">
         <v>922586106</v>
@@ -8498,7 +8501,7 @@
         <v>45701</v>
       </c>
       <c r="J224" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8509,13 +8512,13 @@
         <v>11</v>
       </c>
       <c r="C225" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D225" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E225" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F225" s="0" t="n">
         <v>29032086357</v>
@@ -8530,7 +8533,7 @@
         <v>45475</v>
       </c>
       <c r="J225" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8541,13 +8544,13 @@
         <v>11</v>
       </c>
       <c r="C226" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D226" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E226" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F226" s="0" t="n">
         <v>609237507</v>
@@ -8562,7 +8565,7 @@
         <v>45503</v>
       </c>
       <c r="J226" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8573,13 +8576,13 @@
         <v>11</v>
       </c>
       <c r="C227" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D227" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E227" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F227" s="0" t="n">
         <v>3465228514</v>
@@ -8594,7 +8597,7 @@
         <v>45474</v>
       </c>
       <c r="J227" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8605,7 +8608,7 @@
         <v>11</v>
       </c>
       <c r="C228" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D228" s="0" t="s">
         <v>13</v>
@@ -8626,7 +8629,7 @@
         <v>45543</v>
       </c>
       <c r="J228" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8637,7 +8640,7 @@
         <v>11</v>
       </c>
       <c r="C229" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D229" s="0" t="s">
         <v>13</v>
@@ -8658,7 +8661,7 @@
         <v>45672</v>
       </c>
       <c r="J229" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8669,7 +8672,7 @@
         <v>11</v>
       </c>
       <c r="C230" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D230" s="0" t="s">
         <v>13</v>
@@ -8690,7 +8693,7 @@
         <v>45481</v>
       </c>
       <c r="J230" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8701,7 +8704,7 @@
         <v>11</v>
       </c>
       <c r="C231" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D231" s="0" t="s">
         <v>13</v>
@@ -8722,7 +8725,7 @@
         <v>45603</v>
       </c>
       <c r="J231" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8733,7 +8736,7 @@
         <v>11</v>
       </c>
       <c r="C232" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D232" s="0" t="s">
         <v>13</v>
@@ -8754,7 +8757,7 @@
         <v>45564</v>
       </c>
       <c r="J232" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8765,7 +8768,7 @@
         <v>11</v>
       </c>
       <c r="C233" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D233" s="0" t="s">
         <v>13</v>
@@ -8786,7 +8789,7 @@
         <v>45532</v>
       </c>
       <c r="J233" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Function to return expired offers quantities to the rest of the stock
</commit_message>
<xml_diff>
--- a/proj_aged/core/aged/lab/DataSafeOnes/01_good_AgedStock.xlsx
+++ b/proj_aged/core/aged/lab/DataSafeOnes/01_good_AgedStock.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="393">
   <si>
     <t xml:space="preserve">Plnt</t>
   </si>
@@ -100,9 +100,6 @@
     <t xml:space="preserve">CHO-006-160</t>
   </si>
   <si>
-    <t xml:space="preserve"> ta</t>
-  </si>
-  <si>
     <t xml:space="preserve">96_FU:811NVFAIR-01B_HK buttons 10KG/UC 2</t>
   </si>
   <si>
@@ -1043,9 +1040,6 @@
   </si>
   <si>
     <t xml:space="preserve">MIS-018-328</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOX</t>
   </si>
   <si>
     <t xml:space="preserve">VEN-001-237</t>
@@ -1328,11 +1322,11 @@
   </sheetPr>
   <dimension ref="A1:J233"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G224" activeCellId="0" sqref="G224"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A187" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H201" activeCellId="0" sqref="H201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.37109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.47"/>
@@ -1531,7 +1525,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>10</v>
       </c>
@@ -1554,13 +1548,13 @@
         <v>1640</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="I7" s="2" t="n">
         <v>45566</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1571,7 +1565,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>13</v>
@@ -1603,7 +1597,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>13</v>
@@ -1635,7 +1629,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>13</v>
@@ -1656,7 +1650,7 @@
         <v>45645</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1667,7 +1661,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>13</v>
@@ -1688,7 +1682,7 @@
         <v>45693</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1699,10 +1693,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>35</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>14</v>
@@ -1720,7 +1714,7 @@
         <v>45593</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,10 +1725,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>14</v>
@@ -1752,7 +1746,7 @@
         <v>45633</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1763,13 +1757,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="E14" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>62931743</v>
@@ -1784,7 +1778,7 @@
         <v>45581</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,13 +1789,13 @@
         <v>11</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>86697483</v>
@@ -1816,7 +1810,7 @@
         <v>45680</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,7 +1821,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>13</v>
@@ -1848,7 +1842,7 @@
         <v>45574</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1859,7 +1853,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>13</v>
@@ -1880,7 +1874,7 @@
         <v>45611</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1891,10 +1885,10 @@
         <v>11</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>14</v>
@@ -1912,7 +1906,7 @@
         <v>45603</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1923,10 +1917,10 @@
         <v>11</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>14</v>
@@ -1944,7 +1938,7 @@
         <v>45692</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1955,7 +1949,7 @@
         <v>11</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>13</v>
@@ -1976,7 +1970,7 @@
         <v>45655</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1987,7 +1981,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>13</v>
@@ -2008,7 +2002,7 @@
         <v>45523</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2019,10 +2013,10 @@
         <v>11</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>14</v>
@@ -2040,7 +2034,7 @@
         <v>45641</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2051,10 +2045,10 @@
         <v>11</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>14</v>
@@ -2072,7 +2066,7 @@
         <v>45707</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2083,10 +2077,10 @@
         <v>11</v>
       </c>
       <c r="C24" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>14</v>
@@ -2104,7 +2098,7 @@
         <v>45672</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2115,10 +2109,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>14</v>
@@ -2136,7 +2130,7 @@
         <v>45501</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2147,7 +2141,7 @@
         <v>11</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>13</v>
@@ -2168,7 +2162,7 @@
         <v>45712</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2179,10 +2173,10 @@
         <v>11</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E27" s="0" t="s">
         <v>14</v>
@@ -2200,7 +2194,7 @@
         <v>45594</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2211,10 +2205,10 @@
         <v>11</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>14</v>
@@ -2232,7 +2226,7 @@
         <v>45735</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2243,10 +2237,10 @@
         <v>11</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>14</v>
@@ -2264,7 +2258,7 @@
         <v>45647</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2275,10 +2269,10 @@
         <v>11</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>14</v>
@@ -2296,7 +2290,7 @@
         <v>45739</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2307,10 +2301,10 @@
         <v>11</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>14</v>
@@ -2328,7 +2322,7 @@
         <v>45634</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2339,10 +2333,10 @@
         <v>11</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>14</v>
@@ -2360,7 +2354,7 @@
         <v>45714</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2371,10 +2365,10 @@
         <v>11</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>14</v>
@@ -2392,7 +2386,7 @@
         <v>45601</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2403,7 +2397,7 @@
         <v>11</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>13</v>
@@ -2424,7 +2418,7 @@
         <v>45541</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2435,10 +2429,10 @@
         <v>11</v>
       </c>
       <c r="C35" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>14</v>
@@ -2456,7 +2450,7 @@
         <v>45658</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2467,10 +2461,10 @@
         <v>11</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>14</v>
@@ -2488,7 +2482,7 @@
         <v>45617</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2499,10 +2493,10 @@
         <v>11</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>14</v>
@@ -2520,7 +2514,7 @@
         <v>45641</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2531,10 +2525,10 @@
         <v>11</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>14</v>
@@ -2552,7 +2546,7 @@
         <v>45507</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2563,10 +2557,10 @@
         <v>11</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>14</v>
@@ -2584,7 +2578,7 @@
         <v>45581</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2595,10 +2589,10 @@
         <v>11</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>14</v>
@@ -2616,7 +2610,7 @@
         <v>45580</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2627,10 +2621,10 @@
         <v>11</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>14</v>
@@ -2648,7 +2642,7 @@
         <v>45676</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2659,10 +2653,10 @@
         <v>11</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E42" s="0" t="s">
         <v>14</v>
@@ -2680,7 +2674,7 @@
         <v>45666</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2691,7 +2685,7 @@
         <v>11</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>13</v>
@@ -2712,7 +2706,7 @@
         <v>45656</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2723,10 +2717,10 @@
         <v>11</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E44" s="0" t="s">
         <v>14</v>
@@ -2744,7 +2738,7 @@
         <v>45693</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2755,7 +2749,7 @@
         <v>11</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>13</v>
@@ -2776,7 +2770,7 @@
         <v>45682</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2787,10 +2781,10 @@
         <v>11</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E46" s="0" t="s">
         <v>14</v>
@@ -2808,7 +2802,7 @@
         <v>45628</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2819,10 +2813,10 @@
         <v>11</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E47" s="0" t="s">
         <v>14</v>
@@ -2840,7 +2834,7 @@
         <v>45738</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2851,7 +2845,7 @@
         <v>11</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>13</v>
@@ -2872,7 +2866,7 @@
         <v>45490</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2883,7 +2877,7 @@
         <v>11</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>13</v>
@@ -2904,7 +2898,7 @@
         <v>45692</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2915,7 +2909,7 @@
         <v>11</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>13</v>
@@ -2936,7 +2930,7 @@
         <v>45728</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2947,7 +2941,7 @@
         <v>11</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>13</v>
@@ -2968,7 +2962,7 @@
         <v>45737</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2979,7 +2973,7 @@
         <v>11</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>13</v>
@@ -3000,7 +2994,7 @@
         <v>45666</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3011,7 +3005,7 @@
         <v>11</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>13</v>
@@ -3032,7 +3026,7 @@
         <v>45744</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3043,7 +3037,7 @@
         <v>11</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>13</v>
@@ -3064,7 +3058,7 @@
         <v>45579</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3075,7 +3069,7 @@
         <v>11</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>13</v>
@@ -3096,7 +3090,7 @@
         <v>45495</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3107,7 +3101,7 @@
         <v>11</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>13</v>
@@ -3128,7 +3122,7 @@
         <v>45726</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3139,7 +3133,7 @@
         <v>11</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>13</v>
@@ -3160,7 +3154,7 @@
         <v>45602</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3171,7 +3165,7 @@
         <v>11</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>13</v>
@@ -3192,7 +3186,7 @@
         <v>45486</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3203,7 +3197,7 @@
         <v>11</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>13</v>
@@ -3224,7 +3218,7 @@
         <v>45609</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3235,7 +3229,7 @@
         <v>11</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>13</v>
@@ -3256,7 +3250,7 @@
         <v>45524</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3267,7 +3261,7 @@
         <v>11</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>13</v>
@@ -3288,7 +3282,7 @@
         <v>45745</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3299,7 +3293,7 @@
         <v>11</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>13</v>
@@ -3320,7 +3314,7 @@
         <v>45596</v>
       </c>
       <c r="J62" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3331,7 +3325,7 @@
         <v>11</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>13</v>
@@ -3352,7 +3346,7 @@
         <v>45604</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3363,7 +3357,7 @@
         <v>11</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>13</v>
@@ -3384,7 +3378,7 @@
         <v>45704</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3395,7 +3389,7 @@
         <v>11</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>13</v>
@@ -3416,7 +3410,7 @@
         <v>45554</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3427,7 +3421,7 @@
         <v>11</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>13</v>
@@ -3448,7 +3442,7 @@
         <v>45573</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3459,7 +3453,7 @@
         <v>11</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>13</v>
@@ -3480,7 +3474,7 @@
         <v>45729</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3491,7 +3485,7 @@
         <v>11</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>13</v>
@@ -3512,7 +3506,7 @@
         <v>45611</v>
       </c>
       <c r="J68" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3523,7 +3517,7 @@
         <v>11</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>13</v>
@@ -3544,7 +3538,7 @@
         <v>45731</v>
       </c>
       <c r="J69" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3555,7 +3549,7 @@
         <v>11</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>13</v>
@@ -3576,7 +3570,7 @@
         <v>45487</v>
       </c>
       <c r="J70" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3587,7 +3581,7 @@
         <v>11</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>13</v>
@@ -3608,7 +3602,7 @@
         <v>45546</v>
       </c>
       <c r="J71" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3619,7 +3613,7 @@
         <v>11</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>13</v>
@@ -3640,7 +3634,7 @@
         <v>45578</v>
       </c>
       <c r="J72" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3651,7 +3645,7 @@
         <v>11</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>13</v>
@@ -3672,7 +3666,7 @@
         <v>45696</v>
       </c>
       <c r="J73" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3683,7 +3677,7 @@
         <v>11</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D74" s="0" t="s">
         <v>13</v>
@@ -3704,7 +3698,7 @@
         <v>45528</v>
       </c>
       <c r="J74" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3715,7 +3709,7 @@
         <v>11</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>13</v>
@@ -3736,7 +3730,7 @@
         <v>45574</v>
       </c>
       <c r="J75" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3747,7 +3741,7 @@
         <v>11</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D76" s="0" t="s">
         <v>13</v>
@@ -3768,7 +3762,7 @@
         <v>45583</v>
       </c>
       <c r="J76" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3779,10 +3773,10 @@
         <v>11</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E77" s="0" t="s">
         <v>14</v>
@@ -3800,7 +3794,7 @@
         <v>45566</v>
       </c>
       <c r="J77" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3811,10 +3805,10 @@
         <v>11</v>
       </c>
       <c r="C78" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D78" s="0" t="s">
         <v>135</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>136</v>
       </c>
       <c r="E78" s="0" t="s">
         <v>14</v>
@@ -3832,7 +3826,7 @@
         <v>45682</v>
       </c>
       <c r="J78" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3843,10 +3837,10 @@
         <v>11</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E79" s="0" t="s">
         <v>14</v>
@@ -3864,7 +3858,7 @@
         <v>45737</v>
       </c>
       <c r="J79" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3875,10 +3869,10 @@
         <v>11</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E80" s="0" t="s">
         <v>14</v>
@@ -3896,7 +3890,7 @@
         <v>45525</v>
       </c>
       <c r="J80" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3907,10 +3901,10 @@
         <v>11</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E81" s="0" t="s">
         <v>14</v>
@@ -3928,7 +3922,7 @@
         <v>45712</v>
       </c>
       <c r="J81" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3939,10 +3933,10 @@
         <v>11</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E82" s="0" t="s">
         <v>14</v>
@@ -3960,7 +3954,7 @@
         <v>45612</v>
       </c>
       <c r="J82" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3971,10 +3965,10 @@
         <v>11</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E83" s="0" t="s">
         <v>14</v>
@@ -3992,7 +3986,7 @@
         <v>45740</v>
       </c>
       <c r="J83" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4003,10 +3997,10 @@
         <v>11</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E84" s="0" t="s">
         <v>14</v>
@@ -4024,7 +4018,7 @@
         <v>45669</v>
       </c>
       <c r="J84" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4035,7 +4029,7 @@
         <v>11</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D85" s="0" t="s">
         <v>13</v>
@@ -4056,7 +4050,7 @@
         <v>45736</v>
       </c>
       <c r="J85" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4067,7 +4061,7 @@
         <v>11</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D86" s="0" t="s">
         <v>13</v>
@@ -4088,7 +4082,7 @@
         <v>45667</v>
       </c>
       <c r="J86" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4099,7 +4093,7 @@
         <v>11</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D87" s="0" t="s">
         <v>13</v>
@@ -4120,7 +4114,7 @@
         <v>45641</v>
       </c>
       <c r="J87" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4131,10 +4125,10 @@
         <v>11</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E88" s="0" t="s">
         <v>14</v>
@@ -4152,7 +4146,7 @@
         <v>45513</v>
       </c>
       <c r="J88" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4163,10 +4157,10 @@
         <v>11</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E89" s="0" t="s">
         <v>14</v>
@@ -4184,7 +4178,7 @@
         <v>45586</v>
       </c>
       <c r="J89" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4195,10 +4189,10 @@
         <v>11</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E90" s="0" t="s">
         <v>14</v>
@@ -4216,7 +4210,7 @@
         <v>45661</v>
       </c>
       <c r="J90" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4227,10 +4221,10 @@
         <v>11</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E91" s="0" t="s">
         <v>14</v>
@@ -4248,7 +4242,7 @@
         <v>45696</v>
       </c>
       <c r="J91" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4259,7 +4253,7 @@
         <v>11</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D92" s="0" t="s">
         <v>13</v>
@@ -4280,7 +4274,7 @@
         <v>45553</v>
       </c>
       <c r="J92" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4291,10 +4285,10 @@
         <v>11</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E93" s="0" t="s">
         <v>14</v>
@@ -4312,7 +4306,7 @@
         <v>45557</v>
       </c>
       <c r="J93" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4323,10 +4317,10 @@
         <v>11</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E94" s="0" t="s">
         <v>14</v>
@@ -4344,7 +4338,7 @@
         <v>45559</v>
       </c>
       <c r="J94" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4355,10 +4349,10 @@
         <v>11</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E95" s="0" t="s">
         <v>14</v>
@@ -4376,7 +4370,7 @@
         <v>45590</v>
       </c>
       <c r="J95" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4387,7 +4381,7 @@
         <v>11</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D96" s="0" t="s">
         <v>13</v>
@@ -4408,7 +4402,7 @@
         <v>45509</v>
       </c>
       <c r="J96" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4419,10 +4413,10 @@
         <v>11</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E97" s="0" t="s">
         <v>14</v>
@@ -4440,7 +4434,7 @@
         <v>45637</v>
       </c>
       <c r="J97" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4451,10 +4445,10 @@
         <v>11</v>
       </c>
       <c r="C98" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="D98" s="0" t="s">
         <v>170</v>
-      </c>
-      <c r="D98" s="0" t="s">
-        <v>171</v>
       </c>
       <c r="E98" s="0" t="s">
         <v>14</v>
@@ -4472,7 +4466,7 @@
         <v>45687</v>
       </c>
       <c r="J98" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4483,10 +4477,10 @@
         <v>11</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E99" s="0" t="s">
         <v>14</v>
@@ -4504,7 +4498,7 @@
         <v>45513</v>
       </c>
       <c r="J99" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4515,10 +4509,10 @@
         <v>11</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E100" s="0" t="s">
         <v>14</v>
@@ -4536,7 +4530,7 @@
         <v>45693</v>
       </c>
       <c r="J100" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4547,10 +4541,10 @@
         <v>11</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E101" s="0" t="s">
         <v>14</v>
@@ -4568,7 +4562,7 @@
         <v>45479</v>
       </c>
       <c r="J101" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4579,10 +4573,10 @@
         <v>11</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E102" s="0" t="s">
         <v>14</v>
@@ -4600,7 +4594,7 @@
         <v>45651</v>
       </c>
       <c r="J102" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4611,10 +4605,10 @@
         <v>11</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E103" s="0" t="s">
         <v>14</v>
@@ -4632,7 +4626,7 @@
         <v>45637</v>
       </c>
       <c r="J103" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4643,10 +4637,10 @@
         <v>11</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E104" s="0" t="s">
         <v>14</v>
@@ -4664,7 +4658,7 @@
         <v>45679</v>
       </c>
       <c r="J104" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4675,7 +4669,7 @@
         <v>11</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D105" s="0" t="s">
         <v>13</v>
@@ -4696,7 +4690,7 @@
         <v>45687</v>
       </c>
       <c r="J105" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4707,10 +4701,10 @@
         <v>11</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D106" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E106" s="0" t="s">
         <v>14</v>
@@ -4728,7 +4722,7 @@
         <v>45699</v>
       </c>
       <c r="J106" s="0" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4739,10 +4733,10 @@
         <v>11</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E107" s="0" t="s">
         <v>14</v>
@@ -4760,7 +4754,7 @@
         <v>45596</v>
       </c>
       <c r="J107" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4771,10 +4765,10 @@
         <v>11</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E108" s="0" t="s">
         <v>14</v>
@@ -4792,7 +4786,7 @@
         <v>45659</v>
       </c>
       <c r="J108" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4803,10 +4797,10 @@
         <v>11</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E109" s="0" t="s">
         <v>14</v>
@@ -4824,7 +4818,7 @@
         <v>45614</v>
       </c>
       <c r="J109" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4835,7 +4829,7 @@
         <v>11</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D110" s="0" t="s">
         <v>13</v>
@@ -4856,7 +4850,7 @@
         <v>45510</v>
       </c>
       <c r="J110" s="0" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4867,7 +4861,7 @@
         <v>11</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D111" s="0" t="s">
         <v>13</v>
@@ -4888,7 +4882,7 @@
         <v>45534</v>
       </c>
       <c r="J111" s="0" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4899,10 +4893,10 @@
         <v>11</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E112" s="0" t="s">
         <v>14</v>
@@ -4920,7 +4914,7 @@
         <v>45489</v>
       </c>
       <c r="J112" s="0" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4931,10 +4925,10 @@
         <v>11</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E113" s="0" t="s">
         <v>14</v>
@@ -4952,7 +4946,7 @@
         <v>45582</v>
       </c>
       <c r="J113" s="0" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4963,10 +4957,10 @@
         <v>11</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E114" s="0" t="s">
         <v>14</v>
@@ -4984,7 +4978,7 @@
         <v>45695</v>
       </c>
       <c r="J114" s="0" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4995,7 +4989,7 @@
         <v>11</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D115" s="0" t="s">
         <v>13</v>
@@ -5016,7 +5010,7 @@
         <v>45551</v>
       </c>
       <c r="J115" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5027,10 +5021,10 @@
         <v>11</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E116" s="0" t="s">
         <v>14</v>
@@ -5048,7 +5042,7 @@
         <v>45539</v>
       </c>
       <c r="J116" s="0" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5059,10 +5053,10 @@
         <v>11</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E117" s="0" t="s">
         <v>14</v>
@@ -5080,7 +5074,7 @@
         <v>45656</v>
       </c>
       <c r="J117" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5091,10 +5085,10 @@
         <v>11</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E118" s="0" t="s">
         <v>14</v>
@@ -5112,7 +5106,7 @@
         <v>45505</v>
       </c>
       <c r="J118" s="0" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5123,10 +5117,10 @@
         <v>11</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E119" s="0" t="s">
         <v>14</v>
@@ -5144,7 +5138,7 @@
         <v>45721</v>
       </c>
       <c r="J119" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5155,10 +5149,10 @@
         <v>11</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E120" s="0" t="s">
         <v>14</v>
@@ -5176,7 +5170,7 @@
         <v>45581</v>
       </c>
       <c r="J120" s="0" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5187,7 +5181,7 @@
         <v>11</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D121" s="0" t="s">
         <v>13</v>
@@ -5208,7 +5202,7 @@
         <v>45648</v>
       </c>
       <c r="J121" s="0" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5219,10 +5213,10 @@
         <v>11</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E122" s="0" t="s">
         <v>14</v>
@@ -5240,7 +5234,7 @@
         <v>45661</v>
       </c>
       <c r="J122" s="0" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5251,10 +5245,10 @@
         <v>11</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E123" s="0" t="s">
         <v>14</v>
@@ -5272,7 +5266,7 @@
         <v>45706</v>
       </c>
       <c r="J123" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5283,10 +5277,10 @@
         <v>11</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E124" s="0" t="s">
         <v>14</v>
@@ -5304,7 +5298,7 @@
         <v>45615</v>
       </c>
       <c r="J124" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5315,10 +5309,10 @@
         <v>11</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D125" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E125" s="0" t="s">
         <v>14</v>
@@ -5336,7 +5330,7 @@
         <v>45720</v>
       </c>
       <c r="J125" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5347,10 +5341,10 @@
         <v>11</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D126" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E126" s="0" t="s">
         <v>14</v>
@@ -5368,7 +5362,7 @@
         <v>45659</v>
       </c>
       <c r="J126" s="0" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5379,10 +5373,10 @@
         <v>11</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E127" s="0" t="s">
         <v>14</v>
@@ -5400,7 +5394,7 @@
         <v>45477</v>
       </c>
       <c r="J127" s="0" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5411,10 +5405,10 @@
         <v>11</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E128" s="0" t="s">
         <v>14</v>
@@ -5432,7 +5426,7 @@
         <v>45529</v>
       </c>
       <c r="J128" s="0" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5443,10 +5437,10 @@
         <v>11</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E129" s="0" t="s">
         <v>14</v>
@@ -5464,7 +5458,7 @@
         <v>45566</v>
       </c>
       <c r="J129" s="0" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5475,10 +5469,10 @@
         <v>11</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E130" s="0" t="s">
         <v>14</v>
@@ -5496,7 +5490,7 @@
         <v>45595</v>
       </c>
       <c r="J130" s="0" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5507,10 +5501,10 @@
         <v>11</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E131" s="0" t="s">
         <v>14</v>
@@ -5528,7 +5522,7 @@
         <v>45643</v>
       </c>
       <c r="J131" s="0" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5539,10 +5533,10 @@
         <v>11</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E132" s="0" t="s">
         <v>14</v>
@@ -5560,7 +5554,7 @@
         <v>45701</v>
       </c>
       <c r="J132" s="0" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5571,10 +5565,10 @@
         <v>11</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E133" s="0" t="s">
         <v>14</v>
@@ -5592,7 +5586,7 @@
         <v>45695</v>
       </c>
       <c r="J133" s="0" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5603,10 +5597,10 @@
         <v>11</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D134" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E134" s="0" t="s">
         <v>14</v>
@@ -5624,7 +5618,7 @@
         <v>45573</v>
       </c>
       <c r="J134" s="0" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5635,10 +5629,10 @@
         <v>11</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D135" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E135" s="0" t="s">
         <v>14</v>
@@ -5656,7 +5650,7 @@
         <v>45491</v>
       </c>
       <c r="J135" s="0" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5667,10 +5661,10 @@
         <v>11</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D136" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E136" s="0" t="s">
         <v>14</v>
@@ -5688,7 +5682,7 @@
         <v>45724</v>
       </c>
       <c r="J136" s="0" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5699,10 +5693,10 @@
         <v>11</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D137" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E137" s="0" t="s">
         <v>14</v>
@@ -5720,7 +5714,7 @@
         <v>45702</v>
       </c>
       <c r="J137" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5731,10 +5725,10 @@
         <v>11</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D138" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E138" s="0" t="s">
         <v>14</v>
@@ -5752,7 +5746,7 @@
         <v>45564</v>
       </c>
       <c r="J138" s="0" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5763,10 +5757,10 @@
         <v>11</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D139" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E139" s="0" t="s">
         <v>14</v>
@@ -5784,7 +5778,7 @@
         <v>45740</v>
       </c>
       <c r="J139" s="0" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5795,10 +5789,10 @@
         <v>11</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D140" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E140" s="0" t="s">
         <v>14</v>
@@ -5816,7 +5810,7 @@
         <v>45739</v>
       </c>
       <c r="J140" s="0" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5827,7 +5821,7 @@
         <v>11</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D141" s="0" t="s">
         <v>13</v>
@@ -5848,7 +5842,7 @@
         <v>45537</v>
       </c>
       <c r="J141" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5859,7 +5853,7 @@
         <v>11</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D142" s="0" t="s">
         <v>13</v>
@@ -5880,7 +5874,7 @@
         <v>45644</v>
       </c>
       <c r="J142" s="0" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5891,13 +5885,13 @@
         <v>11</v>
       </c>
       <c r="C143" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="D143" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E143" s="0" t="s">
         <v>246</v>
-      </c>
-      <c r="D143" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E143" s="0" t="s">
-        <v>247</v>
       </c>
       <c r="F143" s="0" t="n">
         <v>922502</v>
@@ -5912,7 +5906,7 @@
         <v>45558</v>
       </c>
       <c r="J143" s="0" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5923,13 +5917,13 @@
         <v>11</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D144" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E144" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F144" s="0" t="n">
         <v>107479977958</v>
@@ -5944,7 +5938,7 @@
         <v>45558</v>
       </c>
       <c r="J144" s="0" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5955,13 +5949,13 @@
         <v>11</v>
       </c>
       <c r="C145" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="D145" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E145" s="0" t="s">
         <v>251</v>
-      </c>
-      <c r="D145" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E145" s="0" t="s">
-        <v>252</v>
       </c>
       <c r="F145" s="0" t="n">
         <v>1513110595</v>
@@ -5976,7 +5970,7 @@
         <v>45512</v>
       </c>
       <c r="J145" s="0" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5987,13 +5981,13 @@
         <v>11</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D146" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E146" s="0" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F146" s="0" t="n">
         <v>3191171</v>
@@ -6008,7 +6002,7 @@
         <v>45561</v>
       </c>
       <c r="J146" s="0" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6019,13 +6013,13 @@
         <v>11</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D147" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E147" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E147" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F147" s="0" t="n">
         <v>62817229110</v>
@@ -6040,7 +6034,7 @@
         <v>45606</v>
       </c>
       <c r="J147" s="0" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6051,13 +6045,13 @@
         <v>11</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D148" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E148" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E148" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F148" s="0" t="n">
         <v>7564700178</v>
@@ -6072,7 +6066,7 @@
         <v>45504</v>
       </c>
       <c r="J148" s="0" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6083,13 +6077,13 @@
         <v>11</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D149" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E149" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E149" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F149" s="0" t="n">
         <v>39315055</v>
@@ -6104,7 +6098,7 @@
         <v>45515</v>
       </c>
       <c r="J149" s="0" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6115,13 +6109,13 @@
         <v>11</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D150" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E150" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E150" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F150" s="0" t="n">
         <v>806341</v>
@@ -6136,7 +6130,7 @@
         <v>45483</v>
       </c>
       <c r="J150" s="0" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6147,13 +6141,13 @@
         <v>11</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D151" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E151" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E151" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F151" s="0" t="n">
         <v>33220182</v>
@@ -6168,7 +6162,7 @@
         <v>45529</v>
       </c>
       <c r="J151" s="0" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6179,13 +6173,13 @@
         <v>11</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D152" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E152" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E152" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F152" s="0" t="n">
         <v>8660373851</v>
@@ -6200,7 +6194,7 @@
         <v>45576</v>
       </c>
       <c r="J152" s="0" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6211,13 +6205,13 @@
         <v>11</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D153" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E153" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E153" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F153" s="0" t="n">
         <v>7173269088</v>
@@ -6232,7 +6226,7 @@
         <v>45708</v>
       </c>
       <c r="J153" s="0" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6243,13 +6237,13 @@
         <v>11</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D154" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E154" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E154" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F154" s="0" t="n">
         <v>76767069</v>
@@ -6264,7 +6258,7 @@
         <v>45563</v>
       </c>
       <c r="J154" s="0" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6275,13 +6269,13 @@
         <v>11</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D155" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E155" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E155" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F155" s="0" t="n">
         <v>564985</v>
@@ -6296,7 +6290,7 @@
         <v>45661</v>
       </c>
       <c r="J155" s="0" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6307,13 +6301,13 @@
         <v>11</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D156" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E156" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E156" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F156" s="0" t="n">
         <v>113017787401</v>
@@ -6328,7 +6322,7 @@
         <v>45519</v>
       </c>
       <c r="J156" s="0" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6339,13 +6333,13 @@
         <v>11</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D157" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E157" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E157" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F157" s="0" t="n">
         <v>6479530310</v>
@@ -6360,7 +6354,7 @@
         <v>45507</v>
       </c>
       <c r="J157" s="0" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6371,13 +6365,13 @@
         <v>11</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D158" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E158" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E158" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F158" s="0" t="n">
         <v>787374</v>
@@ -6392,7 +6386,7 @@
         <v>45690</v>
       </c>
       <c r="J158" s="0" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6403,13 +6397,13 @@
         <v>11</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D159" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E159" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F159" s="0" t="n">
         <v>626885167170</v>
@@ -6424,7 +6418,7 @@
         <v>45532</v>
       </c>
       <c r="J159" s="0" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6435,13 +6429,13 @@
         <v>11</v>
       </c>
       <c r="C160" s="0" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D160" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E160" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F160" s="0" t="n">
         <v>87073583</v>
@@ -6456,7 +6450,7 @@
         <v>45484</v>
       </c>
       <c r="J160" s="0" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6467,13 +6461,13 @@
         <v>11</v>
       </c>
       <c r="C161" s="0" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D161" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E161" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E161" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F161" s="0" t="n">
         <v>676472</v>
@@ -6488,7 +6482,7 @@
         <v>45681</v>
       </c>
       <c r="J161" s="0" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6499,7 +6493,7 @@
         <v>11</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D162" s="0" t="s">
         <v>13</v>
@@ -6520,7 +6514,7 @@
         <v>45540</v>
       </c>
       <c r="J162" s="0" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6531,7 +6525,7 @@
         <v>11</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D163" s="0" t="s">
         <v>13</v>
@@ -6552,7 +6546,7 @@
         <v>45644</v>
       </c>
       <c r="J163" s="0" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6563,10 +6557,10 @@
         <v>11</v>
       </c>
       <c r="C164" s="0" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D164" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E164" s="0" t="s">
         <v>14</v>
@@ -6584,7 +6578,7 @@
         <v>45617</v>
       </c>
       <c r="J164" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6595,10 +6589,10 @@
         <v>11</v>
       </c>
       <c r="C165" s="0" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D165" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E165" s="0" t="s">
         <v>14</v>
@@ -6616,7 +6610,7 @@
         <v>45674</v>
       </c>
       <c r="J165" s="0" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6627,10 +6621,10 @@
         <v>11</v>
       </c>
       <c r="C166" s="0" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D166" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E166" s="0" t="s">
         <v>14</v>
@@ -6648,7 +6642,7 @@
         <v>45479</v>
       </c>
       <c r="J166" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6659,10 +6653,10 @@
         <v>11</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D167" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E167" s="0" t="s">
         <v>14</v>
@@ -6680,7 +6674,7 @@
         <v>45515</v>
       </c>
       <c r="J167" s="0" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6691,10 +6685,10 @@
         <v>11</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E168" s="0" t="s">
         <v>14</v>
@@ -6712,7 +6706,7 @@
         <v>45634</v>
       </c>
       <c r="J168" s="0" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6723,10 +6717,10 @@
         <v>11</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D169" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E169" s="0" t="s">
         <v>14</v>
@@ -6744,7 +6738,7 @@
         <v>45504</v>
       </c>
       <c r="J169" s="0" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6755,7 +6749,7 @@
         <v>11</v>
       </c>
       <c r="C170" s="0" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D170" s="0" t="s">
         <v>13</v>
@@ -6776,7 +6770,7 @@
         <v>45537</v>
       </c>
       <c r="J170" s="0" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6787,10 +6781,10 @@
         <v>11</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D171" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E171" s="0" t="s">
         <v>14</v>
@@ -6808,7 +6802,7 @@
         <v>45527</v>
       </c>
       <c r="J171" s="0" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6819,13 +6813,13 @@
         <v>11</v>
       </c>
       <c r="C172" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="D172" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E172" s="0" t="s">
         <v>293</v>
-      </c>
-      <c r="D172" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E172" s="0" t="s">
-        <v>294</v>
       </c>
       <c r="F172" s="0" t="n">
         <v>206264</v>
@@ -6840,7 +6834,7 @@
         <v>45735</v>
       </c>
       <c r="J172" s="0" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6851,13 +6845,13 @@
         <v>11</v>
       </c>
       <c r="C173" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="D173" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E173" s="0" t="s">
         <v>296</v>
-      </c>
-      <c r="D173" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E173" s="0" t="s">
-        <v>297</v>
       </c>
       <c r="F173" s="0" t="n">
         <v>48066811343</v>
@@ -6872,7 +6866,7 @@
         <v>45658</v>
       </c>
       <c r="J173" s="0" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6883,13 +6877,13 @@
         <v>11</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D174" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E174" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F174" s="0" t="n">
         <v>261476</v>
@@ -6904,7 +6898,7 @@
         <v>45480</v>
       </c>
       <c r="J174" s="0" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6915,13 +6909,13 @@
         <v>11</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D175" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E175" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F175" s="0" t="n">
         <v>311663704102</v>
@@ -6936,7 +6930,7 @@
         <v>45565</v>
       </c>
       <c r="J175" s="0" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6947,13 +6941,13 @@
         <v>11</v>
       </c>
       <c r="C176" s="0" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D176" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E176" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F176" s="0" t="n">
         <v>99085273</v>
@@ -6968,7 +6962,7 @@
         <v>45736</v>
       </c>
       <c r="J176" s="0" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6979,13 +6973,13 @@
         <v>11</v>
       </c>
       <c r="C177" s="0" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D177" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E177" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F177" s="0" t="n">
         <v>491810095347</v>
@@ -7000,7 +6994,7 @@
         <v>45703</v>
       </c>
       <c r="J177" s="0" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7011,13 +7005,13 @@
         <v>11</v>
       </c>
       <c r="C178" s="0" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D178" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E178" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F178" s="0" t="n">
         <v>9595284085</v>
@@ -7032,7 +7026,7 @@
         <v>45538</v>
       </c>
       <c r="J178" s="0" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7043,13 +7037,13 @@
         <v>11</v>
       </c>
       <c r="C179" s="0" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D179" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E179" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F179" s="0" t="n">
         <v>7285382952</v>
@@ -7064,7 +7058,7 @@
         <v>45563</v>
       </c>
       <c r="J179" s="0" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7075,13 +7069,13 @@
         <v>11</v>
       </c>
       <c r="C180" s="0" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D180" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E180" s="0" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F180" s="0" t="n">
         <v>483072700</v>
@@ -7096,7 +7090,7 @@
         <v>45622</v>
       </c>
       <c r="J180" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7107,13 +7101,13 @@
         <v>11</v>
       </c>
       <c r="C181" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="D181" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E181" s="0" t="s">
         <v>311</v>
-      </c>
-      <c r="D181" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E181" s="0" t="s">
-        <v>312</v>
       </c>
       <c r="F181" s="0" t="n">
         <v>951047385</v>
@@ -7128,7 +7122,7 @@
         <v>45601</v>
       </c>
       <c r="J181" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7139,13 +7133,13 @@
         <v>11</v>
       </c>
       <c r="C182" s="0" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D182" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E182" s="0" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F182" s="0" t="n">
         <v>5188981652</v>
@@ -7171,13 +7165,13 @@
         <v>11</v>
       </c>
       <c r="C183" s="0" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D183" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E183" s="0" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F183" s="0" t="n">
         <v>8830053804</v>
@@ -7203,7 +7197,7 @@
         <v>11</v>
       </c>
       <c r="C184" s="0" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D184" s="0" t="s">
         <v>13</v>
@@ -7224,7 +7218,7 @@
         <v>45581</v>
       </c>
       <c r="J184" s="0" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7235,10 +7229,10 @@
         <v>11</v>
       </c>
       <c r="C185" s="0" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D185" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E185" s="0" t="s">
         <v>14</v>
@@ -7256,7 +7250,7 @@
         <v>45655</v>
       </c>
       <c r="J185" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7267,7 +7261,7 @@
         <v>11</v>
       </c>
       <c r="C186" s="0" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D186" s="0" t="s">
         <v>13</v>
@@ -7288,7 +7282,7 @@
         <v>45697</v>
       </c>
       <c r="J186" s="0" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7299,13 +7293,13 @@
         <v>11</v>
       </c>
       <c r="C187" s="0" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D187" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E187" s="0" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F187" s="0" t="n">
         <v>727659058994</v>
@@ -7320,7 +7314,7 @@
         <v>45573</v>
       </c>
       <c r="J187" s="0" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7331,13 +7325,13 @@
         <v>11</v>
       </c>
       <c r="C188" s="0" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D188" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E188" s="0" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F188" s="0" t="n">
         <v>6041531</v>
@@ -7352,7 +7346,7 @@
         <v>45690</v>
       </c>
       <c r="J188" s="0" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7363,13 +7357,13 @@
         <v>11</v>
       </c>
       <c r="C189" s="0" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D189" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E189" s="0" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F189" s="0" t="n">
         <v>8839610860</v>
@@ -7384,7 +7378,7 @@
         <v>45487</v>
       </c>
       <c r="J189" s="0" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7395,13 +7389,13 @@
         <v>11</v>
       </c>
       <c r="C190" s="0" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D190" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E190" s="0" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F190" s="0" t="n">
         <v>10331653</v>
@@ -7416,7 +7410,7 @@
         <v>45634</v>
       </c>
       <c r="J190" s="0" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7427,10 +7421,10 @@
         <v>11</v>
       </c>
       <c r="C191" s="0" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D191" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E191" s="0" t="s">
         <v>14</v>
@@ -7448,7 +7442,7 @@
         <v>45743</v>
       </c>
       <c r="J191" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7459,10 +7453,10 @@
         <v>11</v>
       </c>
       <c r="C192" s="0" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D192" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E192" s="0" t="s">
         <v>14</v>
@@ -7480,7 +7474,7 @@
         <v>45539</v>
       </c>
       <c r="J192" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7491,13 +7485,13 @@
         <v>11</v>
       </c>
       <c r="C193" s="0" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D193" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E193" s="0" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F193" s="0" t="n">
         <v>3011024</v>
@@ -7512,7 +7506,7 @@
         <v>45710</v>
       </c>
       <c r="J193" s="0" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7523,10 +7517,10 @@
         <v>11</v>
       </c>
       <c r="C194" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D194" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E194" s="0" t="s">
         <v>14</v>
@@ -7544,7 +7538,7 @@
         <v>45589</v>
       </c>
       <c r="J194" s="0" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7555,10 +7549,10 @@
         <v>11</v>
       </c>
       <c r="C195" s="0" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D195" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E195" s="0" t="s">
         <v>14</v>
@@ -7576,7 +7570,7 @@
         <v>45648</v>
       </c>
       <c r="J195" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7587,10 +7581,10 @@
         <v>11</v>
       </c>
       <c r="C196" s="0" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D196" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E196" s="0" t="s">
         <v>14</v>
@@ -7608,7 +7602,7 @@
         <v>45557</v>
       </c>
       <c r="J196" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7619,10 +7613,10 @@
         <v>11</v>
       </c>
       <c r="C197" s="0" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D197" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E197" s="0" t="s">
         <v>14</v>
@@ -7640,7 +7634,7 @@
         <v>45665</v>
       </c>
       <c r="J197" s="0" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7651,7 +7645,7 @@
         <v>11</v>
       </c>
       <c r="C198" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D198" s="0" t="s">
         <v>13</v>
@@ -7672,7 +7666,7 @@
         <v>45518</v>
       </c>
       <c r="J198" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7683,7 +7677,7 @@
         <v>11</v>
       </c>
       <c r="C199" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D199" s="0" t="s">
         <v>13</v>
@@ -7704,7 +7698,7 @@
         <v>45539</v>
       </c>
       <c r="J199" s="0" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7715,10 +7709,10 @@
         <v>11</v>
       </c>
       <c r="C200" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D200" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E200" s="0" t="s">
         <v>14</v>
@@ -7736,10 +7730,10 @@
         <v>45547</v>
       </c>
       <c r="J200" s="0" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
         <v>10</v>
       </c>
@@ -7747,13 +7741,13 @@
         <v>11</v>
       </c>
       <c r="C201" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D201" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E201" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F201" s="0" t="n">
         <v>79255121323</v>
@@ -7762,7 +7756,7 @@
         <v>1</v>
       </c>
       <c r="H201" s="0" t="s">
-        <v>341</v>
+        <v>15</v>
       </c>
       <c r="I201" s="2" t="n">
         <v>45559</v>
@@ -7776,13 +7770,13 @@
         <v>11</v>
       </c>
       <c r="C202" s="0" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D202" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E202" s="0" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F202" s="0" t="n">
         <v>1405157491</v>
@@ -7797,7 +7791,7 @@
         <v>45696</v>
       </c>
       <c r="J202" s="0" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7808,13 +7802,13 @@
         <v>11</v>
       </c>
       <c r="C203" s="0" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D203" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E203" s="0" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F203" s="0" t="n">
         <v>6984951</v>
@@ -7829,7 +7823,7 @@
         <v>45483</v>
       </c>
       <c r="J203" s="0" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7840,13 +7834,13 @@
         <v>11</v>
       </c>
       <c r="C204" s="0" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D204" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E204" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F204" s="0" t="n">
         <v>129489134167</v>
@@ -7861,7 +7855,7 @@
         <v>45646</v>
       </c>
       <c r="J204" s="0" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7872,13 +7866,13 @@
         <v>11</v>
       </c>
       <c r="C205" s="0" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D205" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E205" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F205" s="0" t="n">
         <v>29684373</v>
@@ -7893,7 +7887,7 @@
         <v>45546</v>
       </c>
       <c r="J205" s="0" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7904,13 +7898,13 @@
         <v>11</v>
       </c>
       <c r="C206" s="0" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D206" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E206" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F206" s="0" t="n">
         <v>25334895</v>
@@ -7925,7 +7919,7 @@
         <v>45522</v>
       </c>
       <c r="J206" s="0" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7936,13 +7930,13 @@
         <v>11</v>
       </c>
       <c r="C207" s="0" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D207" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E207" s="0" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F207" s="0" t="n">
         <v>8196549819</v>
@@ -7957,7 +7951,7 @@
         <v>45620</v>
       </c>
       <c r="J207" s="0" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7968,13 +7962,13 @@
         <v>11</v>
       </c>
       <c r="C208" s="0" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D208" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E208" s="0" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F208" s="0" t="n">
         <v>186691</v>
@@ -7989,7 +7983,7 @@
         <v>45696</v>
       </c>
       <c r="J208" s="0" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8000,13 +7994,13 @@
         <v>11</v>
       </c>
       <c r="C209" s="0" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D209" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E209" s="0" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F209" s="0" t="n">
         <v>124839445</v>
@@ -8021,7 +8015,7 @@
         <v>45575</v>
       </c>
       <c r="J209" s="0" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8032,13 +8026,13 @@
         <v>11</v>
       </c>
       <c r="C210" s="0" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D210" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E210" s="0" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F210" s="0" t="n">
         <v>589260457</v>
@@ -8053,7 +8047,7 @@
         <v>45671</v>
       </c>
       <c r="J210" s="0" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8064,13 +8058,13 @@
         <v>11</v>
       </c>
       <c r="C211" s="0" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D211" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E211" s="0" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F211" s="0" t="n">
         <v>941190417</v>
@@ -8085,7 +8079,7 @@
         <v>45618</v>
       </c>
       <c r="J211" s="0" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8096,13 +8090,13 @@
         <v>11</v>
       </c>
       <c r="C212" s="0" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D212" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E212" s="0" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F212" s="0" t="n">
         <v>5490867279</v>
@@ -8117,7 +8111,7 @@
         <v>45609</v>
       </c>
       <c r="J212" s="0" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8128,13 +8122,13 @@
         <v>11</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D213" s="0" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E213" s="0" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F213" s="0" t="n">
         <v>73678013427</v>
@@ -8149,7 +8143,7 @@
         <v>45512</v>
       </c>
       <c r="J213" s="0" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8160,13 +8154,13 @@
         <v>11</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D214" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E214" s="0" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F214" s="0" t="n">
         <v>6023391</v>
@@ -8181,7 +8175,7 @@
         <v>45600</v>
       </c>
       <c r="J214" s="0" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8192,13 +8186,13 @@
         <v>11</v>
       </c>
       <c r="C215" s="0" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D215" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E215" s="0" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F215" s="0" t="n">
         <v>598867</v>
@@ -8224,13 +8218,13 @@
         <v>11</v>
       </c>
       <c r="C216" s="0" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D216" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E216" s="0" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F216" s="0" t="n">
         <v>34414881476</v>
@@ -8245,7 +8239,7 @@
         <v>45661</v>
       </c>
       <c r="J216" s="0" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8256,13 +8250,13 @@
         <v>11</v>
       </c>
       <c r="C217" s="0" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D217" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E217" s="0" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F217" s="0" t="n">
         <v>428516229</v>
@@ -8277,7 +8271,7 @@
         <v>45621</v>
       </c>
       <c r="J217" s="0" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8288,13 +8282,13 @@
         <v>11</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D218" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E218" s="0" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F218" s="0" t="n">
         <v>140961878479</v>
@@ -8309,7 +8303,7 @@
         <v>45727</v>
       </c>
       <c r="J218" s="0" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8320,13 +8314,13 @@
         <v>11</v>
       </c>
       <c r="C219" s="0" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D219" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E219" s="0" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F219" s="0" t="n">
         <v>92285640672</v>
@@ -8341,7 +8335,7 @@
         <v>45642</v>
       </c>
       <c r="J219" s="0" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8352,10 +8346,10 @@
         <v>11</v>
       </c>
       <c r="C220" s="0" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D220" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E220" s="0" t="s">
         <v>14</v>
@@ -8373,7 +8367,7 @@
         <v>45503</v>
       </c>
       <c r="J220" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8384,10 +8378,10 @@
         <v>11</v>
       </c>
       <c r="C221" s="0" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D221" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E221" s="0" t="s">
         <v>14</v>
@@ -8405,7 +8399,7 @@
         <v>45586</v>
       </c>
       <c r="J221" s="0" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8416,10 +8410,10 @@
         <v>11</v>
       </c>
       <c r="C222" s="0" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D222" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E222" s="0" t="s">
         <v>14</v>
@@ -8437,7 +8431,7 @@
         <v>45479</v>
       </c>
       <c r="J222" s="0" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8448,10 +8442,10 @@
         <v>11</v>
       </c>
       <c r="C223" s="0" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D223" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E223" s="0" t="s">
         <v>14</v>
@@ -8469,7 +8463,7 @@
         <v>45722</v>
       </c>
       <c r="J223" s="0" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8480,13 +8474,13 @@
         <v>11</v>
       </c>
       <c r="C224" s="0" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D224" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E224" s="0" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F224" s="0" t="n">
         <v>922586106</v>
@@ -8501,7 +8495,7 @@
         <v>45701</v>
       </c>
       <c r="J224" s="0" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8512,13 +8506,13 @@
         <v>11</v>
       </c>
       <c r="C225" s="0" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D225" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E225" s="0" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F225" s="0" t="n">
         <v>29032086357</v>
@@ -8533,7 +8527,7 @@
         <v>45475</v>
       </c>
       <c r="J225" s="0" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8544,13 +8538,13 @@
         <v>11</v>
       </c>
       <c r="C226" s="0" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D226" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E226" s="0" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F226" s="0" t="n">
         <v>609237507</v>
@@ -8565,7 +8559,7 @@
         <v>45503</v>
       </c>
       <c r="J226" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8576,13 +8570,13 @@
         <v>11</v>
       </c>
       <c r="C227" s="0" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D227" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E227" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F227" s="0" t="n">
         <v>3465228514</v>
@@ -8597,7 +8591,7 @@
         <v>45474</v>
       </c>
       <c r="J227" s="0" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8608,7 +8602,7 @@
         <v>11</v>
       </c>
       <c r="C228" s="0" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D228" s="0" t="s">
         <v>13</v>
@@ -8629,7 +8623,7 @@
         <v>45543</v>
       </c>
       <c r="J228" s="0" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8640,7 +8634,7 @@
         <v>11</v>
       </c>
       <c r="C229" s="0" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D229" s="0" t="s">
         <v>13</v>
@@ -8661,7 +8655,7 @@
         <v>45672</v>
       </c>
       <c r="J229" s="0" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8672,7 +8666,7 @@
         <v>11</v>
       </c>
       <c r="C230" s="0" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D230" s="0" t="s">
         <v>13</v>
@@ -8693,7 +8687,7 @@
         <v>45481</v>
       </c>
       <c r="J230" s="0" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8704,7 +8698,7 @@
         <v>11</v>
       </c>
       <c r="C231" s="0" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D231" s="0" t="s">
         <v>13</v>
@@ -8725,7 +8719,7 @@
         <v>45603</v>
       </c>
       <c r="J231" s="0" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8736,7 +8730,7 @@
         <v>11</v>
       </c>
       <c r="C232" s="0" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D232" s="0" t="s">
         <v>13</v>
@@ -8757,7 +8751,7 @@
         <v>45564</v>
       </c>
       <c r="J232" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8768,7 +8762,7 @@
         <v>11</v>
       </c>
       <c r="C233" s="0" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D233" s="0" t="s">
         <v>13</v>
@@ -8789,7 +8783,7 @@
         <v>45532</v>
       </c>
       <c r="J233" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>